<commit_message>
1.update stock_a_indicator_lg for akshare1.9.67
</commit_message>
<xml_diff>
--- a/timeex.xlsx
+++ b/timeex.xlsx
@@ -3523,7 +3523,7 @@
     <t>2023-03-31 00:00:00</t>
   </si>
   <si>
-    <t>2023-04-30 00:00:00</t>
+    <t>2023-04-28 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -3536,7 +3536,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3546,13 +3546,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -4007,46 +4000,49 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4058,103 +4054,101 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -4504,7 +4498,7 @@
   <dimension ref="A1:KO62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -59715,7 +59709,7 @@
       </c>
     </row>
     <row r="62" spans="1:301">
-      <c r="A62" t="s">
+      <c r="A62" s="2" t="s">
         <v>1169</v>
       </c>
       <c r="B62" t="s">

</xml_diff>